<commit_message>
맵 제작 / add
1~5스테이지 제작
</commit_message>
<xml_diff>
--- a/Clean it up! Opossum/Assets/05 DB/StageDB.xlsx
+++ b/Clean it up! Opossum/Assets/05 DB/StageDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Clean-it-up-Opossum\Clean it up! Opossum\Assets\05 DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03628B7E-F99F-4496-9F85-72A1B134C9A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE3F1F-9914-412A-8C83-485BBE144599}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -452,10 +452,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -466,7 +466,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
@@ -488,7 +488,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>